<commit_message>
changes on datepicker class
</commit_message>
<xml_diff>
--- a/tests/src/searchFData.xlsx
+++ b/tests/src/searchFData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">from</t>
   </si>
@@ -28,25 +28,13 @@
     <t xml:space="preserve">to</t>
   </si>
   <si>
-    <t xml:space="preserve">adult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startMonth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startDay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">startYear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">finishMonth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">finishDay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">finishYear</t>
+    <t xml:space="preserve">qty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">startDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finishDate</t>
   </si>
   <si>
     <t xml:space="preserve">LAX</t>
@@ -55,10 +43,10 @@
     <t xml:space="preserve">LAS</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01</t>
+    <t xml:space="preserve">10/01/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/26/2019</t>
   </si>
 </sst>
 </file>
@@ -237,10 +225,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -268,46 +256,22 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>2019</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="H2" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>2019</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
datepicker select startDate ok
</commit_message>
<xml_diff>
--- a/tests/src/searchFData.xlsx
+++ b/tests/src/searchFData.xlsx
@@ -43,10 +43,10 @@
     <t xml:space="preserve">LAS</t>
   </si>
   <si>
-    <t xml:space="preserve">10/01/2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/26/2019</t>
+    <t xml:space="preserve">07/31/2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08/10/2019</t>
   </si>
 </sst>
 </file>
@@ -57,7 +57,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -79,14 +79,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -106,7 +98,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,16 +122,9 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -148,75 +133,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -228,7 +152,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -261,16 +185,16 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>